<commit_message>
Fix for integration test
</commit_message>
<xml_diff>
--- a/cmd/test.xlsx
+++ b/cmd/test.xlsx
@@ -14,36 +14,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
-  <si>
-    <t>Container ID</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Container Name</t>
   </si>
   <si>
-    <t>Status</t>
+    <t>Image Name</t>
   </si>
   <si>
-    <t>IPv4</t>
+    <t>test-import-container</t>
   </si>
   <si>
-    <t>Created At</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>test-x</t>
-  </si>
-  <si>
-    <t>ON</t>
-  </si>
-  <si>
-    <t>172.17.0.99</t>
-  </si>
-  <si>
-    <t>2025-06-30 17:09:52</t>
+    <t>nginx:stable-alpine-perl</t>
   </si>
 </sst>
 </file>
@@ -390,51 +372,30 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="2" width="12.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="2" width="21.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="2" width="23.290714285714284" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="17.25">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+      <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="B2" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="17.25">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>